<commit_message>
Updated test cases for Authoring, Profile, Profile search
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileSearchTestData.xlsx
+++ b/src/test/test-data/ProfileSearchTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="60">
   <si>
     <t>API</t>
   </si>
@@ -97,33 +97,9 @@
     <t>S1_TC_T10</t>
   </si>
   <si>
-    <t>Search for profiles</t>
-  </si>
-  <si>
     <t>1PPROFILESEARCH</t>
   </si>
   <si>
-    <t>GET Profile details</t>
-  </si>
-  <si>
-    <t>search for profiles with names limiting the search results</t>
-  </si>
-  <si>
-    <t>Search for profiles with must containing words with +</t>
-  </si>
-  <si>
-    <t>search for profiles which match the query with wild character.</t>
-  </si>
-  <si>
-    <t>search for profiles which match the query with wild character and should not contain certain words (negative -)</t>
-  </si>
-  <si>
-    <t>search for profiles which match the query with wild character and should not contain multiple words</t>
-  </si>
-  <si>
-    <t>search for profiles and restrict the number of fields returned</t>
-  </si>
-  <si>
     <t>S1_TC_T5</t>
   </si>
   <si>
@@ -136,41 +112,98 @@
     <t>?query=Project&amp;size=1</t>
   </si>
   <si>
+    <t>?query=Project&amp;size=2</t>
+  </si>
+  <si>
+    <t>?query=Proj* -Neon2</t>
+  </si>
+  <si>
+    <t>?query=Project&amp;size=2&amp;fields=category</t>
+  </si>
+  <si>
+    <t>Verify that search for profiles returns 
+results</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for the given hit id, Profile 
+details are returned </t>
+  </si>
+  <si>
+    <t>Verify that for the given hit id, Profile 
+details are returned using query string</t>
+  </si>
+  <si>
+    <t>Verify that for the given hit id and category, Profile 
+details are returned using query string</t>
+  </si>
+  <si>
+    <t>Verify that search for profiles with names and limiting the search results</t>
+  </si>
+  <si>
+    <t>?query=Project</t>
+  </si>
+  <si>
+    <t>?query=Neon1</t>
+  </si>
+  <si>
+    <t>?query=computers</t>
+  </si>
+  <si>
+    <t>?query=QA</t>
+  </si>
+  <si>
+    <t>?query=india</t>
+  </si>
+  <si>
+    <t>S1_TC_T11</t>
+  </si>
+  <si>
+    <t>?query=TR</t>
+  </si>
+  <si>
+    <t>S1_TC_T12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for the given first name in query string, search returns matchedprofiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for the given last name in query string, search returns matchedprofiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for the given interests in query string, search returns matchedprofiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for the given title/role in query string, search returns matchedprofiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for the given country in query string, search returns matchedprofiles </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify that for the given primary institution in query string, search returns matchedprofiles </t>
+  </si>
+  <si>
+    <t>Verify that search for profiles which match the query with wild character and should not contain multiple words</t>
+  </si>
+  <si>
+    <t>S1_TC_T13</t>
+  </si>
+  <si>
+    <t>Verify that search for profiles and restrict the number of fields returned</t>
+  </si>
+  <si>
     <t>status=200||hits.hits._source.firstName=Project//hits.hits._source.lastName=Project</t>
   </si>
   <si>
-    <t>?query=Project&amp;size=2</t>
-  </si>
-  <si>
-    <t>?query=Project+Neon2</t>
-  </si>
-  <si>
-    <t>?query=Proj*</t>
-  </si>
-  <si>
-    <t>?query=Proj* -Neon2</t>
-  </si>
-  <si>
-    <t>?query=Proj* -Neon2 -Neon1</t>
-  </si>
-  <si>
-    <t>?query=Project&amp;size=2&amp;fields=category</t>
-  </si>
-  <si>
     <t>status=200||hits.hits._source.firstName=Project//hits.hist._source.lastName=Project//hits.hits._source.firstName=Neon2//hits.hits._source.lastName=Neon2</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>status=200||hits.hits._source.firstName=Project||hits.hits._source.lastName=Neon1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -229,7 +262,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -243,6 +276,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -538,26 +574,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2:L11"/>
+    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="45.5703125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="54.28515625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="35.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="145.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="41.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="145.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
@@ -598,15 +634,15 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:12">
+    <row r="2" spans="1:12" ht="30">
       <c r="A2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
-        <v>27</v>
+      <c r="B2" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D2" t="s">
         <v>13</v>
@@ -616,29 +652,26 @@
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="K2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12">
+    </row>
+    <row r="3" spans="1:12" ht="30">
       <c r="A3" t="s">
         <v>16</v>
       </c>
-      <c r="B3" t="s">
-        <v>29</v>
+      <c r="B3" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D3" t="s">
         <v>22</v>
@@ -646,29 +679,23 @@
       <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3"/>
-      <c r="G3"/>
       <c r="H3"/>
       <c r="I3" t="s">
         <v>12</v>
       </c>
       <c r="J3" t="s">
-        <v>38</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="30">
       <c r="A4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>29</v>
+      <c r="B4" s="5" t="s">
+        <v>37</v>
       </c>
       <c r="C4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
@@ -676,7 +703,6 @@
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4"/>
       <c r="G4" t="s">
         <v>18</v>
       </c>
@@ -685,22 +711,18 @@
         <v>12</v>
       </c>
       <c r="J4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45">
       <c r="A5" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>29</v>
+      <c r="B5" s="6" t="s">
+        <v>38</v>
       </c>
       <c r="C5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s">
         <v>17</v>
@@ -708,7 +730,6 @@
       <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5"/>
       <c r="G5" t="s">
         <v>20</v>
       </c>
@@ -717,22 +738,18 @@
         <v>12</v>
       </c>
       <c r="J5" t="s">
-        <v>38</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" ht="45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="30">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D6" t="s">
         <v>13</v>
@@ -740,18 +757,12 @@
       <c r="E6" t="s">
         <v>1</v>
       </c>
-      <c r="F6"/>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
       <c r="H6"/>
-      <c r="I6"/>
       <c r="J6" t="s">
-        <v>40</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:12" ht="45">
@@ -759,10 +770,10 @@
         <v>23</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>31</v>
+        <v>48</v>
       </c>
       <c r="C7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
         <v>13</v>
@@ -770,18 +781,12 @@
       <c r="E7" t="s">
         <v>1</v>
       </c>
-      <c r="F7"/>
       <c r="G7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="H7"/>
-      <c r="I7"/>
       <c r="J7" t="s">
-        <v>47</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>49</v>
+        <v>58</v>
       </c>
     </row>
     <row r="8" spans="1:12" ht="45">
@@ -789,10 +794,10 @@
         <v>24</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>32</v>
+        <v>49</v>
       </c>
       <c r="C8" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
         <v>13</v>
@@ -800,29 +805,23 @@
       <c r="E8" t="s">
         <v>1</v>
       </c>
-      <c r="F8"/>
       <c r="G8" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H8"/>
-      <c r="I8"/>
       <c r="J8" t="s">
-        <v>40</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="75">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="45">
       <c r="A9" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="C9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
         <v>13</v>
@@ -830,29 +829,23 @@
       <c r="E9" t="s">
         <v>1</v>
       </c>
-      <c r="F9"/>
       <c r="G9" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H9"/>
-      <c r="I9"/>
       <c r="J9" t="s">
-        <v>40</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="60">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="45">
       <c r="A10" t="s">
         <v>25</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D10" t="s">
         <v>13</v>
@@ -860,18 +853,12 @@
       <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="F10"/>
       <c r="G10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H10"/>
-      <c r="I10"/>
       <c r="J10" t="s">
-        <v>38</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>49</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11" spans="1:12" ht="45">
@@ -879,10 +866,10 @@
         <v>26</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>35</v>
+        <v>52</v>
       </c>
       <c r="C11" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D11" t="s">
         <v>13</v>
@@ -890,18 +877,84 @@
       <c r="E11" t="s">
         <v>1</v>
       </c>
-      <c r="F11"/>
       <c r="G11" t="s">
+        <v>44</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="45">
+      <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
         <v>46</v>
       </c>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11" t="s">
-        <v>38</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>49</v>
+      <c r="H12"/>
+      <c r="J12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="60">
+      <c r="A13" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>13</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>33</v>
+      </c>
+      <c r="H13"/>
+      <c r="J13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="30">
+      <c r="A14" t="s">
+        <v>55</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14"/>
+      <c r="J14" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added new testcases in Authoring, updated test case ids in Authoring, Profile and ProfileSearch.
</commit_message>
<xml_diff>
--- a/src/test/test-data/ProfileSearchTestData.xlsx
+++ b/src/test/test-data/ProfileSearchTestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="58">
   <si>
     <t>API</t>
   </si>
@@ -52,9 +52,6 @@
     <t>STORE</t>
   </si>
   <si>
-    <t>S1_TC_T1</t>
-  </si>
-  <si>
     <t>/search</t>
   </si>
   <si>
@@ -64,48 +61,12 @@
     <t>hits.hits._id</t>
   </si>
   <si>
-    <t>S1_TC_T2</t>
-  </si>
-  <si>
     <t>/details</t>
   </si>
   <si>
-    <t>?id=(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>S1_TC_T3</t>
-  </si>
-  <si>
-    <t>?id=(S1_TC_T1_hits.hits._id)&amp;fields=category</t>
-  </si>
-  <si>
-    <t>S1_TC_T4</t>
-  </si>
-  <si>
-    <t>/details/(S1_TC_T1_hits.hits._id)</t>
-  </si>
-  <si>
-    <t>S1_TC_T6</t>
-  </si>
-  <si>
-    <t>S1_TC_T7</t>
-  </si>
-  <si>
-    <t>S1_TC_T9</t>
-  </si>
-  <si>
-    <t>S1_TC_T10</t>
-  </si>
-  <si>
     <t>1PPROFILESEARCH</t>
   </si>
   <si>
-    <t>S1_TC_T5</t>
-  </si>
-  <si>
-    <t>S1_TC_T8</t>
-  </si>
-  <si>
     <t>status=200</t>
   </si>
   <si>
@@ -130,9 +91,6 @@
     <t>?query=india</t>
   </si>
   <si>
-    <t>S1_TC_T11</t>
-  </si>
-  <si>
     <t>?query=TR</t>
   </si>
   <si>
@@ -145,9 +103,6 @@
     <t>status=200||hits.hits._source.firstName=Project||hits.hits._source.lastName=Neon1</t>
   </si>
   <si>
-    <t>Verify that user is able to search profiles</t>
-  </si>
-  <si>
     <t>Verify that user is able to get Profile details</t>
   </si>
   <si>
@@ -172,25 +127,73 @@
     <t>Verify that user is able to search for profiles and restrict the number of fields returned</t>
   </si>
   <si>
-    <t>Verify that for the given hit id and category, Profile 
-details are returned using query string in API</t>
-  </si>
-  <si>
-    <t>Verify that for the given hit id, Profile 
-details are returned using query string in API</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t>PASS</t>
+    <t>Verify that for the given hit id and category, Profile details are returned using query string in API</t>
+  </si>
+  <si>
+    <t>OPQA-699</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles with Last name</t>
+  </si>
+  <si>
+    <t>?query=API AUTOMATION</t>
+  </si>
+  <si>
+    <t>status=200||hits.hits._source.firstName=Project||hits.hits._source.lastName=Neon2||hits.hits._source.interest[0]=API AUTOMATION</t>
+  </si>
+  <si>
+    <t>OPQA-434</t>
+  </si>
+  <si>
+    <t>/details/(OPQA-434_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-434_hits.hits._id)</t>
+  </si>
+  <si>
+    <t>?id=(OPQA-434_hits.hits._id)&amp;fields=category</t>
+  </si>
+  <si>
+    <t>Verify that user is able to search for profiles</t>
+  </si>
+  <si>
+    <t>OPQA-435</t>
+  </si>
+  <si>
+    <t>OPQA-698</t>
+  </si>
+  <si>
+    <t>Verify that for the given hit id, Profile details are returned using query string in API</t>
+  </si>
+  <si>
+    <t>OPQA-437</t>
+  </si>
+  <si>
+    <t>OPQA-436</t>
+  </si>
+  <si>
+    <t>OPQA-438</t>
+  </si>
+  <si>
+    <t>OPQA-439</t>
+  </si>
+  <si>
+    <t>OPQA-440</t>
+  </si>
+  <si>
+    <t>OPQA-441</t>
+  </si>
+  <si>
+    <t>OPQA-442</t>
+  </si>
+  <si>
+    <t>OPQA-443</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -294,14 +297,12 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -600,36 +601,36 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:L12"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="10.42578125" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="35.7109375" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="8.85546875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="41.5703125" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" style="5" width="15.5703125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="145.42578125" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="24.7109375" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="1" max="1" width="10.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="35.7109375" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="17.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="30.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="8.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="20" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="41.5703125" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="15.5703125" style="5" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="145.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="24.7109375" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="10.7109375" bestFit="1" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="C1" s="6" t="s">
         <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -648,7 +649,7 @@
         <v>9</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="J1" s="2" t="s">
         <v>10</v>
@@ -661,339 +662,302 @@
       </c>
     </row>
     <row r="2" spans="1:12" ht="31.5">
-      <c r="A2" t="s">
+      <c r="A2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
         <v>12</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D2" t="s">
-        <v>13</v>
       </c>
       <c r="E2" s="1" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="1"/>
       <c r="G2" s="1" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="1"/>
       <c r="J2" t="s">
-        <v>40</v>
+        <v>26</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="L2" t="s">
-        <v>55</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:12" ht="31.5">
-      <c r="A3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="C3" t="s">
-        <v>27</v>
+      <c r="A3" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D3" t="s">
-        <v>22</v>
+        <v>43</v>
       </c>
       <c r="E3" t="s">
         <v>1</v>
       </c>
-      <c r="F3"/>
-      <c r="G3"/>
       <c r="H3"/>
       <c r="I3" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3"/>
-      <c r="L3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="45">
-      <c r="A4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>53</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="47.25">
+      <c r="A4" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
         <v>1</v>
       </c>
-      <c r="F4"/>
       <c r="G4" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="H4"/>
       <c r="I4" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4"/>
-      <c r="L4" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" ht="60">
-      <c r="A5" t="s">
-        <v>21</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="45">
+      <c r="A5" s="8" t="s">
+        <v>38</v>
       </c>
       <c r="B5" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>16</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E5" t="s">
         <v>1</v>
       </c>
-      <c r="F5"/>
       <c r="G5" t="s">
-        <v>20</v>
+        <v>45</v>
       </c>
       <c r="H5"/>
       <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="31.5">
+      <c r="A6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" t="s">
         <v>12</v>
       </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5"/>
-      <c r="L5" t="s">
+      <c r="E6" t="s">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>21</v>
+      </c>
+      <c r="H6"/>
+      <c r="J6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="31.5">
+      <c r="A7" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7"/>
+      <c r="J7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="31.5">
+      <c r="A8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1</v>
+      </c>
+      <c r="G8" t="s">
+        <v>40</v>
+      </c>
+      <c r="H8"/>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="31.5">
+      <c r="A9" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H9"/>
+      <c r="J9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" ht="31.5">
+      <c r="A10" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="B10" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C10" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1</v>
+      </c>
+      <c r="G10" t="s">
+        <v>24</v>
+      </c>
+      <c r="H10"/>
+      <c r="J10" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" ht="31.5">
+      <c r="A11" s="8" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="31.5">
-      <c r="A6" t="s">
+      <c r="B11" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1</v>
+      </c>
+      <c r="G11" t="s">
+        <v>25</v>
+      </c>
+      <c r="H11"/>
+      <c r="J11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="63">
+      <c r="A12" s="8" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1</v>
+      </c>
+      <c r="G12" t="s">
+        <v>19</v>
+      </c>
+      <c r="H12"/>
+      <c r="J12" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D6" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" t="s">
-        <v>1</v>
-      </c>
-      <c r="F6"/>
-      <c r="G6" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6"/>
-      <c r="I6"/>
-      <c r="J6" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6"/>
-      <c r="L6" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" ht="31.5">
-      <c r="A7" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="C7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" t="s">
-        <v>13</v>
-      </c>
-      <c r="E7" t="s">
-        <v>1</v>
-      </c>
-      <c r="F7"/>
-      <c r="G7" t="s">
-        <v>35</v>
-      </c>
-      <c r="H7"/>
-      <c r="I7"/>
-      <c r="J7" t="s">
-        <v>42</v>
-      </c>
-      <c r="K7"/>
-      <c r="L7" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" ht="31.5">
-      <c r="A8" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="C8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D8" t="s">
-        <v>13</v>
-      </c>
-      <c r="E8" t="s">
-        <v>1</v>
-      </c>
-      <c r="F8"/>
-      <c r="G8" t="s">
+    </row>
+    <row r="13" spans="1:12" ht="47.25">
+      <c r="A13" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B13" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="H8"/>
-      <c r="I8"/>
-      <c r="J8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8"/>
-      <c r="L8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" ht="31.5">
-      <c r="A9" t="s">
-        <v>29</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C9" t="s">
-        <v>27</v>
-      </c>
-      <c r="D9" t="s">
-        <v>13</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9"/>
-      <c r="G9" t="s">
-        <v>37</v>
-      </c>
-      <c r="H9"/>
-      <c r="I9"/>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9"/>
-      <c r="L9" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" ht="31.5">
-      <c r="A10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B10" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="C10" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" t="s">
-        <v>13</v>
-      </c>
-      <c r="E10" t="s">
-        <v>1</v>
-      </c>
-      <c r="F10"/>
-      <c r="G10" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10"/>
-      <c r="I10"/>
-      <c r="J10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10"/>
-      <c r="L10" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" ht="63">
-      <c r="A11" t="s">
-        <v>26</v>
-      </c>
-      <c r="B11" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="C11" t="s">
-        <v>27</v>
-      </c>
-      <c r="D11" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" t="s">
-        <v>1</v>
-      </c>
-      <c r="F11"/>
-      <c r="G11" t="s">
-        <v>32</v>
-      </c>
-      <c r="H11"/>
-      <c r="I11"/>
-      <c r="J11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K11"/>
-      <c r="L11" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" ht="47.25">
-      <c r="A12" t="s">
-        <v>38</v>
-      </c>
-      <c r="B12" s="8" t="s">
-        <v>51</v>
-      </c>
-      <c r="C12" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" t="s">
-        <v>1</v>
-      </c>
-      <c r="F12"/>
-      <c r="G12" t="s">
-        <v>33</v>
-      </c>
-      <c r="H12"/>
-      <c r="I12"/>
-      <c r="J12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12"/>
-      <c r="L12" t="s">
-        <v>55</v>
+      <c r="C13" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1</v>
+      </c>
+      <c r="G13" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13"/>
+      <c r="J13" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>